<commit_message>
canada prophet, prophet commonality changes
</commit_message>
<xml_diff>
--- a/results/Pred_Hackathon_2023_Somnolence_09052023.xlsx
+++ b/results/Pred_Hackathon_2023_Somnolence_09052023.xlsx
@@ -140,7 +140,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -150,10 +150,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -177,7 +173,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -205,6 +201,15 @@
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="B3" s="0" t="n">
+        <v>7.072981</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>8.051687</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>6.04784</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -253,13 +258,13 @@
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="2" t="n">
         <v>4.166677</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9" s="2" t="n">
         <v>5.479863</v>
       </c>
-      <c r="D9" s="3" t="n">
+      <c r="D9" s="1" t="n">
         <v>2.856417</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ger ita jpn prophet
</commit_message>
<xml_diff>
--- a/results/Pred_Hackathon_2023_Somnolence_09052023.xlsx
+++ b/results/Pred_Hackathon_2023_Somnolence_09052023.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
   <si>
     <t xml:space="preserve">UNEMPLYMENT_RATE</t>
   </si>
@@ -37,19 +37,25 @@
     <t xml:space="preserve">Lower Bound</t>
   </si>
   <si>
+    <t xml:space="preserve">Targeted Month for Prediction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source model</t>
+  </si>
+  <si>
     <t xml:space="preserve">Canada</t>
   </si>
   <si>
+    <t xml:space="preserve">May</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prophet CV</t>
+  </si>
+  <si>
     <t xml:space="preserve">France</t>
   </si>
   <si>
-    <t xml:space="preserve">6.991768</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7.241449</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.729585</t>
+    <t xml:space="preserve">April</t>
   </si>
   <si>
     <t xml:space="preserve">Germany</t>
@@ -62,6 +68,9 @@
   </si>
   <si>
     <t xml:space="preserve">United Kingdom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March</t>
   </si>
   <si>
     <t xml:space="preserve">United States</t>
@@ -170,20 +179,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -196,53 +205,116 @@
       <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="n">
         <v>7.072981</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="2" t="n">
         <v>8.051687</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="2" t="n">
         <v>6.04784</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>6.991768</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>7.241449</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>6.729585</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>3.1088488</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>3.344162</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>2.851482</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F5" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>8.14796</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>8.513808</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>7.817619</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F6" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>2.008909</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>2.293228</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>2.013057</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B8" s="2" t="n">
         <v>3.385219</v>
@@ -253,10 +325,16 @@
       <c r="D8" s="2" t="n">
         <v>2.973279</v>
       </c>
+      <c r="E8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B9" s="2" t="n">
         <v>4.166677</v>
@@ -266,6 +344,12 @@
       </c>
       <c r="D9" s="1" t="n">
         <v>2.856417</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>